<commit_message>
Se agregan direcciones de Dealers
</commit_message>
<xml_diff>
--- a/datos_entrada/Pedidos_Externos.XLSX
+++ b/datos_entrada/Pedidos_Externos.XLSX
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rcarrero\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05A33DA8-0766-4911-A095-7F9106A6E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="14940"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -936,7 +937,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1286,42 +1287,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>280</v>
       </c>
@@ -1401,7 +1406,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1486,7 @@
         <v>0.65901620370369995</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1566,7 @@
         <v>0.41322916666666998</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1641,7 +1646,7 @@
         <v>0.67962962962963003</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1726,7 @@
         <v>0.65372685185184998</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1801,7 +1806,7 @@
         <v>0.37378472222221998</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1881,7 +1886,7 @@
         <v>0.37378472222221998</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1961,7 +1966,7 @@
         <v>0.37378472222221998</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2041,7 +2046,7 @@
         <v>0.63130787037036995</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2121,7 +2126,7 @@
         <v>0.85304398148147997</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2201,7 +2206,7 @@
         <v>0.66528935185185001</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>0.66471064814814995</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2366,7 @@
         <v>0.66413194444444001</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2441,7 +2446,7 @@
         <v>0.66331018518519003</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2521,7 +2526,7 @@
         <v>0.65781250000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2601,7 +2606,7 @@
         <v>0.65175925925926004</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2681,7 +2686,7 @@
         <v>0.65175925925926004</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2761,7 +2766,7 @@
         <v>0.63928240740741005</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2841,7 +2846,7 @@
         <v>0.63928240740741005</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2921,7 +2926,7 @@
         <v>0.63928240740741005</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -3001,7 +3006,7 @@
         <v>0.63831018518519</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3081,7 +3086,7 @@
         <v>0.58924768518519</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>0.58844907407406999</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3241,7 +3246,7 @@
         <v>0.58466435185184995</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3321,7 +3326,7 @@
         <v>0.54090277777777995</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3401,7 +3406,7 @@
         <v>0.54084490740740998</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3481,7 +3486,7 @@
         <v>0.54084490740740998</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3561,7 +3566,7 @@
         <v>0.53974537037036996</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3641,7 +3646,7 @@
         <v>0.53796296296295998</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -3721,7 +3726,7 @@
         <v>0.53796296296295998</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -3801,7 +3806,7 @@
         <v>0.53796296296295998</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -3881,7 +3886,7 @@
         <v>0.53062500000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -3961,7 +3966,7 @@
         <v>0.52979166666666999</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>0.52888888888888996</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -4121,7 +4126,7 @@
         <v>0.52276620370369997</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -4201,7 +4206,7 @@
         <v>0.52222222222222003</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -4281,7 +4286,7 @@
         <v>0.52222222222222003</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -4361,7 +4366,7 @@
         <v>0.52222222222222003</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -4441,7 +4446,7 @@
         <v>0.46969907407407002</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -4521,7 +4526,7 @@
         <v>0.43473379629629999</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -4601,7 +4606,7 @@
         <v>0.41574074074074002</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -4681,7 +4686,7 @@
         <v>0.41574074074074002</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -4761,7 +4766,7 @@
         <v>0.41574074074074002</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -4841,7 +4846,7 @@
         <v>0.41468749999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -4921,7 +4926,7 @@
         <v>0.41034722222221998</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -5001,7 +5006,7 @@
         <v>0.40966435185185002</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -5081,7 +5086,7 @@
         <v>0.39885416666667001</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -5161,7 +5166,7 @@
         <v>0.39802083333332999</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -5241,7 +5246,7 @@
         <v>0.39802083333332999</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -5321,7 +5326,7 @@
         <v>0.39597222222222</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>25</v>
       </c>
@@ -5401,7 +5406,7 @@
         <v>0.39364583333332998</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -5481,7 +5486,7 @@
         <v>0.39364583333332998</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -5561,7 +5566,7 @@
         <v>0.37251157407406998</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -5641,7 +5646,7 @@
         <v>0.36420138888888998</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -5721,7 +5726,7 @@
         <v>0.36306712962963</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -5801,7 +5806,7 @@
         <v>0.36306712962963</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -5881,7 +5886,7 @@
         <v>0.36306712962963</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -5961,7 +5966,7 @@
         <v>0.31657407407407001</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -6041,7 +6046,7 @@
         <v>0.31565972222222</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>210</v>
       </c>
@@ -6121,7 +6126,7 @@
         <v>0.66358796296295997</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>210</v>
       </c>
@@ -6201,7 +6206,7 @@
         <v>0.66358796296295997</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>210</v>
       </c>
@@ -6281,7 +6286,7 @@
         <v>0.66358796296295997</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>210</v>
       </c>
@@ -6361,7 +6366,7 @@
         <v>0.62659722222222003</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>210</v>
       </c>
@@ -6441,7 +6446,7 @@
         <v>0.62453703703704</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>210</v>
       </c>
@@ -6521,7 +6526,7 @@
         <v>0.62453703703704</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>210</v>
       </c>
@@ -6601,7 +6606,7 @@
         <v>0.58560185185184999</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>210</v>
       </c>
@@ -6681,7 +6686,7 @@
         <v>0.39881944444444001</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>210</v>
       </c>
@@ -6761,7 +6766,7 @@
         <v>0.39881944444444001</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>210</v>
       </c>
@@ -6841,7 +6846,7 @@
         <v>0.39853009259258998</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>210</v>
       </c>
@@ -6921,7 +6926,7 @@
         <v>0.39841435185184998</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -7001,7 +7006,7 @@
         <v>0.39841435185184998</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>210</v>
       </c>
@@ -7081,7 +7086,7 @@
         <v>0.39841435185184998</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>210</v>
       </c>
@@ -7161,7 +7166,7 @@
         <v>0.39615740740741001</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>210</v>
       </c>
@@ -7241,7 +7246,7 @@
         <v>0.34984953703704003</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>210</v>
       </c>
@@ -7321,7 +7326,7 @@
         <v>0.34984953703704003</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -7401,7 +7406,7 @@
         <v>0.34976851851851998</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>210</v>
       </c>
@@ -7481,7 +7486,7 @@
         <v>0.32221064814814998</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>210</v>
       </c>
@@ -7561,7 +7566,7 @@
         <v>0.31954861111110999</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>210</v>
       </c>
@@ -7641,7 +7646,7 @@
         <v>0.31954861111110999</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>210</v>
       </c>
@@ -7721,7 +7726,7 @@
         <v>0.31954861111110999</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>210</v>
       </c>
@@ -7801,7 +7806,7 @@
         <v>0.29793981481481002</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>210</v>
       </c>
@@ -7881,7 +7886,7 @@
         <v>0.29589120370369998</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>210</v>
       </c>
@@ -7961,7 +7966,7 @@
         <v>0.77819444444443997</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>210</v>
       </c>
@@ -8041,7 +8046,7 @@
         <v>0.77767361111111</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>210</v>
       </c>
@@ -8121,7 +8126,7 @@
         <v>0.77709490740741005</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -8201,7 +8206,7 @@
         <v>0.75239583333333004</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>210</v>
       </c>
@@ -8281,7 +8286,7 @@
         <v>0.75142361111111</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>210</v>
       </c>

</xml_diff>